<commit_message>
02-05-2025 - 12:41 - JCSantos - Antes de incorporar el flujo de Dani.
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JCSantos\Documents\UiPath\Contraportada_RPA\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1D09911-FB3C-4096-9FEF-5891D7EB3F69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC52D0F5-2778-4FEE-8771-14DD1C3D151A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8895" yWindow="3780" windowWidth="27690" windowHeight="12900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8895" yWindow="3780" windowWidth="27690" windowHeight="17220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="58">
   <si>
     <t>Name</t>
   </si>
@@ -180,6 +180,24 @@
   </si>
   <si>
     <t>EXCEL;Chrome;PlanMaker</t>
+  </si>
+  <si>
+    <t>PromptChatGPT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Actúa como un experto en literatura. A partir de la siguiente consulta de un usuario (filtrada previamente para asegurar que esté relacionada con recomendaciones de libros), responde con un único objeto JSON que represente un libro relevante. Solo debes rellenar los campos mencionados en la consulta: si el usuario menciona un título, rellena solo el campo 'titulo'; si menciona un autor, rellena 'autor'; si menciona un tema, estilo o género, inclúyelo en 'sinopsis' copiando exactamente esos términos (máximo 5 palabras, sin añadir o modificar nada); si proporciona varios datos, completa todos los que estén presentes. Los campos disponibles son: 'titulo', 'autor', 'isbn', 'editorial', 'sinopsis'. Deja vacíos los campos no mencionados. Si la consulta no proporciona información suficiente, responde con este JSON: { 'SL-01': 'El contenido del correo es insuficiente para realizar la búsqueda de libros' }. Si la consulta no está relacionada con libros o está incompleta, responde con este JSON: { 'SL-02': 'Contenido de correo no corresponde con consulta de libros' } No agregues ningún texto fuera del JSON. Solo responde con el objeto JSON o el objeto de error, según corresponda. Consulta del usuario:  </t>
+  </si>
+  <si>
+    <t>urlChatGPT</t>
+  </si>
+  <si>
+    <t>urlTodosTusLibros</t>
+  </si>
+  <si>
+    <t>https://chatgpt.com/</t>
+  </si>
+  <si>
+    <t>https://www.todostuslibros.com/buscador_avanzado</t>
   </si>
 </sst>
 </file>
@@ -231,7 +249,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -241,6 +259,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -558,7 +577,7 @@
   <dimension ref="A1:Z999"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -648,7 +667,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="10" spans="1:26" ht="14.25" customHeight="1">
+    <row r="10" spans="1:26" ht="12.75" customHeight="1">
       <c r="A10" t="s">
         <v>49</v>
       </c>
@@ -656,7 +675,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="11" spans="1:26" ht="14.25" customHeight="1">
+    <row r="11" spans="1:26" ht="14.25" hidden="1" customHeight="1">
       <c r="A11" t="s">
         <v>44</v>
       </c>
@@ -664,9 +683,30 @@
         <v>51</v>
       </c>
     </row>
-    <row r="12" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="13" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="14" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="12" spans="1:26" s="3" customFormat="1">
+      <c r="A12" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="13" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A13" t="s">
+        <v>54</v>
+      </c>
+      <c r="B13" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="14" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A14" t="s">
+        <v>55</v>
+      </c>
+      <c r="B14" t="s">
+        <v>57</v>
+      </c>
+    </row>
     <row r="15" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="16" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="17" ht="14.25" customHeight="1"/>

</xml_diff>

<commit_message>
2-Mayo-2025 - JCSantos . Módulo Dani consulta libros.
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JCSantos\Documents\UiPath\Contraportada_RPA\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC52D0F5-2778-4FEE-8771-14DD1C3D151A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D85B809A-50EC-4136-AEF8-A6A09D91E3D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8895" yWindow="3780" windowWidth="27690" windowHeight="17220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6480" yWindow="2895" windowWidth="29700" windowHeight="17220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -577,7 +577,7 @@
   <dimension ref="A1:Z999"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -675,7 +675,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="11" spans="1:26" ht="14.25" hidden="1" customHeight="1">
+    <row r="11" spans="1:26">
       <c r="A11" t="s">
         <v>44</v>
       </c>

</xml_diff>

<commit_message>
4-5-2025 - 13:37 - JCSantos - Optimización.
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JCSantos\Documents\UiPath\Contraportada_RPA\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D85B809A-50EC-4136-AEF8-A6A09D91E3D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07D4B2FC-8DF3-41D1-B598-A1D2B81BCF63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6480" yWindow="2895" windowWidth="29700" windowHeight="17220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1950" yWindow="1950" windowWidth="28800" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -185,9 +185,6 @@
     <t>PromptChatGPT</t>
   </si>
   <si>
-    <t xml:space="preserve">Actúa como un experto en literatura. A partir de la siguiente consulta de un usuario (filtrada previamente para asegurar que esté relacionada con recomendaciones de libros), responde con un único objeto JSON que represente un libro relevante. Solo debes rellenar los campos mencionados en la consulta: si el usuario menciona un título, rellena solo el campo 'titulo'; si menciona un autor, rellena 'autor'; si menciona un tema, estilo o género, inclúyelo en 'sinopsis' copiando exactamente esos términos (máximo 5 palabras, sin añadir o modificar nada); si proporciona varios datos, completa todos los que estén presentes. Los campos disponibles son: 'titulo', 'autor', 'isbn', 'editorial', 'sinopsis'. Deja vacíos los campos no mencionados. Si la consulta no proporciona información suficiente, responde con este JSON: { 'SL-01': 'El contenido del correo es insuficiente para realizar la búsqueda de libros' }. Si la consulta no está relacionada con libros o está incompleta, responde con este JSON: { 'SL-02': 'Contenido de correo no corresponde con consulta de libros' } No agregues ningún texto fuera del JSON. Solo responde con el objeto JSON o el objeto de error, según corresponda. Consulta del usuario:  </t>
-  </si>
-  <si>
     <t>urlChatGPT</t>
   </si>
   <si>
@@ -198,6 +195,9 @@
   </si>
   <si>
     <t>https://www.todostuslibros.com/buscador_avanzado</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Actúa como un experto en literatura. A partir de la siguiente consulta de un usuario (filtrada previamente para asegurar que esté relacionada con recomendaciones de libros), responde con un único objeto JSON que represente un libro relevante. Solo debes rellenar los campos mencionados en la consulta: si el usuario menciona un título, rellena solo el campo 'titulo'; si menciona un autor, rellena 'autor'; si menciona un tema, estilo o género, inclúyelo en 'sinopsis' copiando exactamente esos términos (máximo 5 palabras, sin añadir o modificar nada); si proporciona varios datos, completa todos los que estén presentes. Los campos disponibles son: 'titulo', 'autor', 'isbn', 'editorial', 'sinopsis'. Es obligatorio mostrar todos los campos. Deja vacíos los campos no mencionados. Si la consulta no proporciona información suficiente, responde con este JSON: { 'SL-01': 'El contenido del correo es insuficiente para realizar la búsqueda de libros' }. Si la consulta no está relacionada con libros o está incompleta, responde con este JSON: { 'SL-02': 'Contenido de correo no corresponde con consulta de libros' } No agregues ningún texto fuera del JSON. Solo responde con el objeto JSON o el objeto de error, según corresponda. Consulta del usuario:  </t>
   </si>
 </sst>
 </file>
@@ -688,23 +688,23 @@
         <v>52</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="14.25" customHeight="1">
       <c r="A13" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B13" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="14" spans="1:26" ht="14.25" customHeight="1">
       <c r="A14" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B14" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="15" spans="1:26" ht="14.25" customHeight="1"/>

</xml_diff>